<commit_message>
add 1/13/20 CEI data
</commit_message>
<xml_diff>
--- a/data/tle/2020-01-13_CEI.xlsx
+++ b/data/tle/2020-01-13_CEI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrcunning/Projects/bsrte/data/tle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1EBEA8-7A47-3B4B-82E2-509F2904085F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A5B6E7F-B51B-564A-B2DB-8D15B06D4B79}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="16020" xr2:uid="{16BF75F0-FE87-2549-9CA0-5E2987E2B2F5}"/>
+    <workbookView xWindow="10060" yWindow="1240" windowWidth="27640" windowHeight="16020" xr2:uid="{16BF75F0-FE87-2549-9CA0-5E2987E2B2F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="180">
   <si>
     <t>Name</t>
   </si>
@@ -187,9 +187,6 @@
   </si>
   <si>
     <t>11,2,1</t>
-  </si>
-  <si>
-    <t>10,1</t>
   </si>
   <si>
     <t>missing</t>
@@ -809,19 +806,19 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1138,8 +1135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{343B95AD-90F0-0645-82C2-72AE1B8F65F0}">
   <dimension ref="A1:AJ1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF3" sqref="AF3:AJ3"/>
+    <sheetView tabSelected="1" topLeftCell="U9" workbookViewId="0">
+      <selection activeCell="AC26" sqref="AC26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1182,246 +1179,246 @@
       <c r="B1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="31"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="34"/>
       <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="32" t="s">
-        <v>180</v>
-      </c>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="31"/>
+        <v>179</v>
+      </c>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="34"/>
       <c r="M1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="N1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="31"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="34"/>
       <c r="S1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="T1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="31"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="34"/>
       <c r="Y1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="Z1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="AA1" s="30"/>
-      <c r="AB1" s="30"/>
-      <c r="AC1" s="30"/>
-      <c r="AD1" s="31"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="34"/>
       <c r="AE1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="AF1" s="32" t="s">
-        <v>180</v>
-      </c>
-      <c r="AG1" s="30"/>
-      <c r="AH1" s="30"/>
-      <c r="AI1" s="30"/>
-      <c r="AJ1" s="31"/>
+        <v>179</v>
+      </c>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="33"/>
+      <c r="AJ1" s="34"/>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="29">
+      <c r="B2" s="35">
         <v>43843</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="31"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="34"/>
       <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="29">
+      <c r="H2" s="35">
         <v>43843</v>
       </c>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="31"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="34"/>
       <c r="M2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="29">
+      <c r="N2" s="35">
         <v>43843</v>
       </c>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="31"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="34"/>
       <c r="S2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="T2" s="29">
+      <c r="T2" s="35">
         <v>43843</v>
       </c>
-      <c r="U2" s="30"/>
-      <c r="V2" s="30"/>
-      <c r="W2" s="30"/>
-      <c r="X2" s="31"/>
+      <c r="U2" s="33"/>
+      <c r="V2" s="33"/>
+      <c r="W2" s="33"/>
+      <c r="X2" s="34"/>
       <c r="Y2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Z2" s="29">
+      <c r="Z2" s="35">
         <v>43843</v>
       </c>
-      <c r="AA2" s="30"/>
-      <c r="AB2" s="30"/>
-      <c r="AC2" s="30"/>
-      <c r="AD2" s="31"/>
+      <c r="AA2" s="33"/>
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="34"/>
       <c r="AE2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AF2" s="29">
+      <c r="AF2" s="35">
         <v>43843</v>
       </c>
-      <c r="AG2" s="30"/>
-      <c r="AH2" s="30"/>
-      <c r="AI2" s="30"/>
-      <c r="AJ2" s="31"/>
+      <c r="AG2" s="33"/>
+      <c r="AH2" s="33"/>
+      <c r="AI2" s="33"/>
+      <c r="AJ2" s="34"/>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>179</v>
-      </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="31"/>
+        <v>178</v>
+      </c>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="34"/>
       <c r="G3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H3" s="32" t="s">
-        <v>179</v>
-      </c>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="31"/>
+        <v>178</v>
+      </c>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="34"/>
       <c r="M3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="N3" s="32" t="s">
-        <v>179</v>
-      </c>
-      <c r="O3" s="30"/>
-      <c r="P3" s="30"/>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="31"/>
+        <v>178</v>
+      </c>
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="34"/>
       <c r="S3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="T3" s="32" t="s">
-        <v>179</v>
-      </c>
-      <c r="U3" s="30"/>
-      <c r="V3" s="30"/>
-      <c r="W3" s="30"/>
-      <c r="X3" s="31"/>
+        <v>178</v>
+      </c>
+      <c r="U3" s="33"/>
+      <c r="V3" s="33"/>
+      <c r="W3" s="33"/>
+      <c r="X3" s="34"/>
       <c r="Y3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="Z3" s="32" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA3" s="30"/>
-      <c r="AB3" s="30"/>
-      <c r="AC3" s="30"/>
-      <c r="AD3" s="31"/>
+        <v>178</v>
+      </c>
+      <c r="AA3" s="33"/>
+      <c r="AB3" s="33"/>
+      <c r="AC3" s="33"/>
+      <c r="AD3" s="34"/>
       <c r="AE3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="AF3" s="32" t="s">
-        <v>179</v>
-      </c>
-      <c r="AG3" s="30"/>
-      <c r="AH3" s="30"/>
-      <c r="AI3" s="30"/>
-      <c r="AJ3" s="31"/>
+        <v>178</v>
+      </c>
+      <c r="AG3" s="33"/>
+      <c r="AH3" s="33"/>
+      <c r="AI3" s="33"/>
+      <c r="AJ3" s="34"/>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="33">
+      <c r="B4" s="29">
         <v>139</v>
       </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="35"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="31"/>
       <c r="G4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="33">
+      <c r="H4" s="29">
         <v>140</v>
       </c>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="35"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="31"/>
       <c r="M4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="N4" s="33">
+      <c r="N4" s="29">
         <v>141</v>
       </c>
-      <c r="O4" s="34"/>
-      <c r="P4" s="34"/>
-      <c r="Q4" s="34"/>
-      <c r="R4" s="35"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="31"/>
       <c r="S4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="T4" s="33">
+      <c r="T4" s="29">
         <v>142</v>
       </c>
-      <c r="U4" s="34"/>
-      <c r="V4" s="34"/>
-      <c r="W4" s="34"/>
-      <c r="X4" s="35"/>
+      <c r="U4" s="30"/>
+      <c r="V4" s="30"/>
+      <c r="W4" s="30"/>
+      <c r="X4" s="31"/>
       <c r="Y4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="Z4" s="33">
+      <c r="Z4" s="29">
         <v>143</v>
       </c>
-      <c r="AA4" s="34"/>
-      <c r="AB4" s="34"/>
-      <c r="AC4" s="34"/>
-      <c r="AD4" s="35"/>
+      <c r="AA4" s="30"/>
+      <c r="AB4" s="30"/>
+      <c r="AC4" s="30"/>
+      <c r="AD4" s="31"/>
       <c r="AE4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="AF4" s="33">
+      <c r="AF4" s="29">
         <v>144</v>
       </c>
-      <c r="AG4" s="34"/>
-      <c r="AH4" s="34"/>
-      <c r="AI4" s="34"/>
-      <c r="AJ4" s="35"/>
+      <c r="AG4" s="30"/>
+      <c r="AH4" s="30"/>
+      <c r="AI4" s="30"/>
+      <c r="AJ4" s="31"/>
     </row>
     <row r="5" spans="1:36" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -1550,7 +1547,7 @@
         <v>8</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>11</v>
@@ -1568,7 +1565,7 @@
         <v>8</v>
       </c>
       <c r="L6" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M6" s="18">
         <v>133</v>
@@ -1577,7 +1574,7 @@
         <v>8</v>
       </c>
       <c r="O6" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P6" s="5">
         <v>134</v>
@@ -1604,7 +1601,7 @@
         <v>8</v>
       </c>
       <c r="X6" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Y6" s="18">
         <v>133</v>
@@ -1622,7 +1619,7 @@
         <v>1</v>
       </c>
       <c r="AD6" s="24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE6" s="4" t="s">
         <v>11</v>
@@ -1631,7 +1628,7 @@
         <v>8</v>
       </c>
       <c r="AG6" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AH6" s="4" t="s">
         <v>12</v>
@@ -1640,7 +1637,7 @@
         <v>8</v>
       </c>
       <c r="AJ6" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:36" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1649,35 +1646,35 @@
         <v>15</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J7" s="7"/>
       <c r="K7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M7" s="6"/>
       <c r="N7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="O7" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P7" s="8"/>
       <c r="Q7" s="9">
@@ -1691,7 +1688,7 @@
         <v>15</v>
       </c>
       <c r="U7" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="V7" s="7"/>
       <c r="W7" s="3" t="s">
@@ -1712,21 +1709,21 @@
         <v>2</v>
       </c>
       <c r="AD7" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AE7" s="7"/>
       <c r="AF7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="AG7" s="13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AH7" s="7"/>
       <c r="AI7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="AJ7" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:36" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1735,35 +1732,35 @@
         <v>20</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="3" t="s">
         <v>20</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="3" t="s">
         <v>20</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J8" s="7"/>
       <c r="K8" s="3" t="s">
         <v>20</v>
       </c>
       <c r="L8" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M8" s="6"/>
       <c r="N8" s="3" t="s">
         <v>20</v>
       </c>
       <c r="O8" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="P8" s="8"/>
       <c r="Q8" s="9">
@@ -1784,35 +1781,35 @@
         <v>20</v>
       </c>
       <c r="X8" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Y8" s="6"/>
       <c r="Z8" s="3" t="s">
         <v>20</v>
       </c>
       <c r="AA8" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AB8" s="8"/>
       <c r="AC8" s="9">
         <v>3</v>
       </c>
       <c r="AD8" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AE8" s="7"/>
       <c r="AF8" s="3" t="s">
         <v>20</v>
       </c>
       <c r="AG8" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AH8" s="7"/>
       <c r="AI8" s="3" t="s">
         <v>20</v>
       </c>
       <c r="AJ8" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:36" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1821,28 +1818,28 @@
         <v>22</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="3" t="s">
         <v>22</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="3" t="s">
         <v>22</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J9" s="7"/>
       <c r="K9" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L9" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M9" s="6"/>
       <c r="N9" s="3" t="s">
@@ -1884,14 +1881,14 @@
         <v>4</v>
       </c>
       <c r="AD9" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AE9" s="7"/>
       <c r="AF9" s="3" t="s">
         <v>22</v>
       </c>
       <c r="AG9" s="13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AH9" s="7"/>
       <c r="AI9" s="3" t="s">
@@ -1914,21 +1911,21 @@
         <v>23</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="10" t="s">
         <v>23</v>
       </c>
       <c r="I10" s="26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J10" s="7"/>
       <c r="K10" s="3" t="s">
         <v>23</v>
       </c>
       <c r="L10" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M10" s="6"/>
       <c r="N10" s="10" t="s">
@@ -1942,21 +1939,21 @@
         <v>5</v>
       </c>
       <c r="R10" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S10" s="7"/>
       <c r="T10" s="10" t="s">
         <v>23</v>
       </c>
       <c r="U10" s="26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="V10" s="7"/>
       <c r="W10" s="3" t="s">
         <v>23</v>
       </c>
       <c r="X10" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Y10" s="6"/>
       <c r="Z10" s="10" t="s">
@@ -1970,7 +1967,7 @@
         <v>5</v>
       </c>
       <c r="AD10" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AE10" s="7"/>
       <c r="AF10" s="10" t="s">
@@ -1984,7 +1981,7 @@
         <v>23</v>
       </c>
       <c r="AJ10" s="13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:36" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2013,7 +2010,7 @@
         <v>8</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>31</v>
@@ -2022,7 +2019,7 @@
         <v>8</v>
       </c>
       <c r="L11" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M11" s="19">
         <v>125</v>
@@ -2040,7 +2037,7 @@
         <v>1</v>
       </c>
       <c r="R11" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="S11" s="3" t="s">
         <v>30</v>
@@ -2049,7 +2046,7 @@
         <v>8</v>
       </c>
       <c r="U11" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="V11" s="3" t="s">
         <v>31</v>
@@ -2058,7 +2055,7 @@
         <v>8</v>
       </c>
       <c r="X11" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Y11" s="19">
         <v>125</v>
@@ -2085,7 +2082,7 @@
         <v>8</v>
       </c>
       <c r="AG11" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AH11" s="3" t="s">
         <v>31</v>
@@ -2094,7 +2091,7 @@
         <v>8</v>
       </c>
       <c r="AJ11" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:36" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2117,7 +2114,7 @@
         <v>15</v>
       </c>
       <c r="I12" s="27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J12" s="7"/>
       <c r="K12" s="3" t="s">
@@ -2145,14 +2142,14 @@
         <v>15</v>
       </c>
       <c r="U12" s="27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="V12" s="7"/>
       <c r="W12" s="3" t="s">
         <v>15</v>
       </c>
       <c r="X12" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Y12" s="6"/>
       <c r="Z12" s="12" t="s">
@@ -2166,21 +2163,21 @@
         <v>2</v>
       </c>
       <c r="AD12" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AE12" s="7"/>
       <c r="AF12" s="12" t="s">
         <v>15</v>
       </c>
       <c r="AG12" s="27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AH12" s="7"/>
       <c r="AI12" s="3" t="s">
         <v>15</v>
       </c>
       <c r="AJ12" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:36" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2259,14 +2256,14 @@
         <v>20</v>
       </c>
       <c r="AG13" s="13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AH13" s="7"/>
       <c r="AI13" s="3" t="s">
         <v>20</v>
       </c>
       <c r="AJ13" s="13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:36" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2275,7 +2272,7 @@
         <v>22</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="3" t="s">
@@ -2296,7 +2293,7 @@
         <v>22</v>
       </c>
       <c r="L14" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M14" s="6"/>
       <c r="N14" s="3" t="s">
@@ -2317,14 +2314,14 @@
         <v>22</v>
       </c>
       <c r="U14" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="V14" s="7"/>
       <c r="W14" s="3" t="s">
         <v>22</v>
       </c>
       <c r="X14" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Y14" s="6"/>
       <c r="Z14" s="3" t="s">
@@ -2345,14 +2342,14 @@
         <v>22</v>
       </c>
       <c r="AG14" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AH14" s="7"/>
       <c r="AI14" s="3" t="s">
         <v>22</v>
       </c>
       <c r="AJ14" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:36" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2361,7 +2358,7 @@
         <v>23</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="3" t="s">
@@ -2375,14 +2372,14 @@
         <v>23</v>
       </c>
       <c r="I15" s="26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J15" s="7"/>
       <c r="K15" s="3" t="s">
         <v>23</v>
       </c>
       <c r="L15" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M15" s="6"/>
       <c r="N15" s="10" t="s">
@@ -2403,14 +2400,14 @@
         <v>23</v>
       </c>
       <c r="U15" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="V15" s="7"/>
       <c r="W15" s="3" t="s">
         <v>23</v>
       </c>
       <c r="X15" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Y15" s="6"/>
       <c r="Z15" s="10" t="s">
@@ -2431,14 +2428,14 @@
         <v>23</v>
       </c>
       <c r="AG15" s="26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AH15" s="7"/>
       <c r="AI15" s="3" t="s">
         <v>23</v>
       </c>
       <c r="AJ15" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16" spans="1:36" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2449,7 +2446,7 @@
         <v>8</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>40</v>
@@ -2458,7 +2455,7 @@
         <v>8</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>41</v>
@@ -2485,7 +2482,7 @@
         <v>8</v>
       </c>
       <c r="O16" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P16" s="9">
         <v>95</v>
@@ -2494,7 +2491,7 @@
         <v>1</v>
       </c>
       <c r="R16" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="S16" s="3" t="s">
         <v>41</v>
@@ -2503,7 +2500,7 @@
         <v>8</v>
       </c>
       <c r="U16" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="V16" s="3" t="s">
         <v>42</v>
@@ -2521,7 +2518,7 @@
         <v>8</v>
       </c>
       <c r="AA16" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AB16" s="9">
         <v>95</v>
@@ -2530,7 +2527,7 @@
         <v>1</v>
       </c>
       <c r="AD16" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AE16" s="3" t="s">
         <v>41</v>
@@ -2539,7 +2536,7 @@
         <v>8</v>
       </c>
       <c r="AG16" s="13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AH16" s="3" t="s">
         <v>42</v>
@@ -2548,7 +2545,7 @@
         <v>8</v>
       </c>
       <c r="AJ16" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:36" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2557,14 +2554,14 @@
         <v>15</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="3" t="s">
         <v>15</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G17" s="7"/>
       <c r="H17" s="12" t="s">
@@ -2583,14 +2580,14 @@
         <v>15</v>
       </c>
       <c r="O17" s="25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P17" s="8"/>
       <c r="Q17" s="9">
         <v>2</v>
       </c>
       <c r="R17" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="S17" s="7"/>
       <c r="T17" s="12" t="s">
@@ -2611,14 +2608,14 @@
         <v>15</v>
       </c>
       <c r="AA17" s="25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AB17" s="8"/>
       <c r="AC17" s="9">
         <v>2</v>
       </c>
       <c r="AD17" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AE17" s="7"/>
       <c r="AF17" s="12" t="s">
@@ -2641,21 +2638,21 @@
         <v>20</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="3" t="s">
         <v>20</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G18" s="7"/>
       <c r="H18" s="3" t="s">
         <v>20</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J18" s="7"/>
       <c r="K18" s="3" t="s">
@@ -2667,14 +2664,14 @@
         <v>20</v>
       </c>
       <c r="O18" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P18" s="8"/>
       <c r="Q18" s="9">
         <v>3</v>
       </c>
       <c r="R18" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S18" s="7"/>
       <c r="T18" s="3" t="s">
@@ -2695,21 +2692,21 @@
         <v>20</v>
       </c>
       <c r="AA18" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AB18" s="8"/>
       <c r="AC18" s="9">
         <v>3</v>
       </c>
       <c r="AD18" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AE18" s="7"/>
       <c r="AF18" s="3" t="s">
         <v>20</v>
       </c>
       <c r="AG18" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AH18" s="7"/>
       <c r="AI18" s="3" t="s">
@@ -2725,21 +2722,21 @@
         <v>22</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="3" t="s">
         <v>22</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G19" s="7"/>
       <c r="H19" s="3" t="s">
         <v>22</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J19" s="7"/>
       <c r="K19" s="3" t="s">
@@ -2751,21 +2748,21 @@
         <v>22</v>
       </c>
       <c r="O19" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P19" s="8"/>
       <c r="Q19" s="9">
         <v>4</v>
       </c>
       <c r="R19" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="S19" s="7"/>
       <c r="T19" s="3" t="s">
         <v>22</v>
       </c>
       <c r="U19" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="V19" s="7"/>
       <c r="W19" s="3" t="s">
@@ -2779,14 +2776,14 @@
         <v>22</v>
       </c>
       <c r="AA19" s="25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AB19" s="8"/>
       <c r="AC19" s="9">
         <v>4</v>
       </c>
       <c r="AD19" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AE19" s="7"/>
       <c r="AF19" s="3" t="s">
@@ -2800,7 +2797,7 @@
         <v>22</v>
       </c>
       <c r="AJ19" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:36" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2809,14 +2806,14 @@
         <v>23</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G20" s="7"/>
       <c r="H20" s="10" t="s">
@@ -2835,21 +2832,21 @@
         <v>23</v>
       </c>
       <c r="O20" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="P20" s="11"/>
       <c r="Q20" s="9">
         <v>5</v>
       </c>
       <c r="R20" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="S20" s="7"/>
       <c r="T20" s="10" t="s">
         <v>23</v>
       </c>
       <c r="U20" s="26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="V20" s="7"/>
       <c r="W20" s="3" t="s">
@@ -2863,14 +2860,14 @@
         <v>23</v>
       </c>
       <c r="AA20" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AB20" s="11"/>
       <c r="AC20" s="9">
         <v>5</v>
       </c>
       <c r="AD20" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AE20" s="7"/>
       <c r="AF20" s="10" t="s">
@@ -2884,7 +2881,7 @@
         <v>23</v>
       </c>
       <c r="AJ20" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:36" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2895,7 +2892,7 @@
         <v>8</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>48</v>
@@ -2913,7 +2910,7 @@
         <v>8</v>
       </c>
       <c r="I21" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>50</v>
@@ -2931,7 +2928,7 @@
         <v>8</v>
       </c>
       <c r="O21" s="25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="P21" s="9" t="s">
         <v>48</v>
@@ -2967,16 +2964,16 @@
         <v>8</v>
       </c>
       <c r="AA21" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AB21" s="9" t="s">
         <v>48</v>
       </c>
       <c r="AC21" s="9" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="AD21" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AE21" s="3" t="s">
         <v>49</v>
@@ -2985,7 +2982,7 @@
         <v>8</v>
       </c>
       <c r="AG21" s="13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AH21" s="3" t="s">
         <v>50</v>
@@ -3003,14 +3000,14 @@
         <v>15</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="3" t="s">
         <v>15</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G22" s="7"/>
       <c r="H22" s="12" t="s">
@@ -3031,7 +3028,7 @@
         <v>15</v>
       </c>
       <c r="O22" s="25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P22" s="8"/>
       <c r="Q22" s="9">
@@ -3059,14 +3056,14 @@
         <v>15</v>
       </c>
       <c r="AA22" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AB22" s="8"/>
       <c r="AC22" s="9" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="AD22" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AE22" s="7"/>
       <c r="AF22" s="12" t="s">
@@ -3089,21 +3086,21 @@
         <v>20</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="3" t="s">
         <v>20</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G23" s="7"/>
       <c r="H23" s="3" t="s">
         <v>20</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J23" s="7"/>
       <c r="K23" s="3" t="s">
@@ -3117,7 +3114,7 @@
         <v>20</v>
       </c>
       <c r="O23" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P23" s="8"/>
       <c r="Q23" s="9">
@@ -3131,7 +3128,7 @@
         <v>20</v>
       </c>
       <c r="U23" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="V23" s="7"/>
       <c r="W23" s="3" t="s">
@@ -3145,14 +3142,14 @@
         <v>20</v>
       </c>
       <c r="AA23" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AB23" s="8"/>
       <c r="AC23" s="9" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="AD23" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AE23" s="7"/>
       <c r="AF23" s="3" t="s">
@@ -3175,21 +3172,21 @@
         <v>22</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="3" t="s">
         <v>22</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G24" s="7"/>
       <c r="H24" s="3" t="s">
         <v>22</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J24" s="7"/>
       <c r="K24" s="3" t="s">
@@ -3203,7 +3200,7 @@
         <v>22</v>
       </c>
       <c r="O24" s="25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="P24" s="8"/>
       <c r="Q24" s="9">
@@ -3217,7 +3214,7 @@
         <v>22</v>
       </c>
       <c r="U24" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="V24" s="7"/>
       <c r="W24" s="3" t="s">
@@ -3231,7 +3228,7 @@
         <v>22</v>
       </c>
       <c r="AA24" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB24" s="8"/>
       <c r="AC24" s="9" t="s">
@@ -3245,7 +3242,7 @@
         <v>22</v>
       </c>
       <c r="AG24" s="13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AH24" s="7"/>
       <c r="AI24" s="3" t="s">
@@ -3261,21 +3258,21 @@
         <v>23</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G25" s="7"/>
       <c r="H25" s="10" t="s">
         <v>23</v>
       </c>
       <c r="I25" s="26" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J25" s="7"/>
       <c r="K25" s="3" t="s">
@@ -3289,7 +3286,7 @@
         <v>23</v>
       </c>
       <c r="O25" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="P25" s="11"/>
       <c r="Q25" s="9">
@@ -3303,7 +3300,7 @@
         <v>23</v>
       </c>
       <c r="U25" s="26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="V25" s="7"/>
       <c r="W25" s="3" t="s">
@@ -3317,14 +3314,14 @@
         <v>23</v>
       </c>
       <c r="AA25" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AB25" s="11"/>
       <c r="AC25" s="9" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="AD25" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AE25" s="7"/>
       <c r="AF25" s="10" t="s">
@@ -3343,7 +3340,7 @@
     </row>
     <row r="26" spans="1:36" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>8</v>
@@ -3352,14 +3349,14 @@
         <v>9</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>8</v>
       </c>
       <c r="F26" s="14"/>
       <c r="G26" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>8</v>
@@ -3368,7 +3365,7 @@
         <v>25</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>8</v>
@@ -3377,23 +3374,23 @@
         <v>9</v>
       </c>
       <c r="M26" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N26" s="3" t="s">
         <v>8</v>
       </c>
       <c r="O26" s="25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="P26" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q26" s="9">
         <v>1</v>
       </c>
       <c r="R26" s="9"/>
       <c r="S26" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="T26" s="3" t="s">
         <v>8</v>
@@ -3402,7 +3399,7 @@
         <v>45</v>
       </c>
       <c r="V26" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="W26" s="3" t="s">
         <v>8</v>
@@ -3411,23 +3408,23 @@
         <v>20</v>
       </c>
       <c r="Y26" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Z26" s="3" t="s">
         <v>8</v>
       </c>
       <c r="AA26" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AB26" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AC26" s="9">
         <v>1</v>
       </c>
       <c r="AD26" s="9"/>
       <c r="AE26" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AF26" s="3" t="s">
         <v>8</v>
@@ -3436,7 +3433,7 @@
         <v>9</v>
       </c>
       <c r="AH26" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AI26" s="3" t="s">
         <v>8</v>
@@ -3477,7 +3474,7 @@
         <v>15</v>
       </c>
       <c r="O27" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P27" s="7"/>
       <c r="Q27" s="3" t="s">
@@ -3557,7 +3554,7 @@
         <v>20</v>
       </c>
       <c r="O28" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="P28" s="7"/>
       <c r="Q28" s="3" t="s">
@@ -3602,7 +3599,7 @@
         <v>20</v>
       </c>
       <c r="AJ28" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="29" spans="1:36" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3637,7 +3634,7 @@
         <v>22</v>
       </c>
       <c r="O29" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="P29" s="7"/>
       <c r="Q29" s="10" t="s">
@@ -5287,6 +5284,18 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="AF2:AJ2"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="N1:R1"/>
+    <mergeCell ref="T1:X1"/>
+    <mergeCell ref="Z1:AD1"/>
+    <mergeCell ref="AF1:AJ1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="N2:R2"/>
+    <mergeCell ref="T2:X2"/>
+    <mergeCell ref="Z2:AD2"/>
     <mergeCell ref="AF4:AJ4"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="H3:L3"/>
@@ -5299,18 +5308,6 @@
     <mergeCell ref="N4:R4"/>
     <mergeCell ref="T4:X4"/>
     <mergeCell ref="Z4:AD4"/>
-    <mergeCell ref="AF2:AJ2"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="N1:R1"/>
-    <mergeCell ref="T1:X1"/>
-    <mergeCell ref="Z1:AD1"/>
-    <mergeCell ref="AF1:AJ1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="N2:R2"/>
-    <mergeCell ref="T2:X2"/>
-    <mergeCell ref="Z2:AD2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>